<commit_message>
Added table to DB excel file
</commit_message>
<xml_diff>
--- a/Table_AttributeNames.xlsx
+++ b/Table_AttributeNames.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Suguru/Documents/Java_Programming/IT353_Project/Proj353/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Desktop/Netbeans/Proj353x/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
+    <sheet name="Submissions" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,12 +28,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Attribute</t>
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Datatype</t>
+  </si>
+  <si>
+    <t>USERID</t>
+  </si>
+  <si>
+    <t>VARCHAR(15)</t>
+  </si>
+  <si>
+    <t>NUMBER</t>
+  </si>
+  <si>
+    <t>SUBMISSIONID(PK)</t>
+  </si>
+  <si>
+    <t>RATING</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>SUBMISSION_DATE</t>
   </si>
 </sst>
 </file>
@@ -389,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -551,4 +576,190 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>